<commit_message>
updated CAH to new forecasting method
</commit_message>
<xml_diff>
--- a/CAH FTL/volume_forecaster/Define Matching Weeks.xlsx
+++ b/CAH FTL/volume_forecaster/Define Matching Weeks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amfam-my.sharepoint.com/personal/sierra_steiner_connectbyamfam_com/Documents/Documents/FTL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{31271D5B-B40D-45F2-898B-D61F0B1B82E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F9475F6-4750-4DD6-A406-96FFDE7379B5}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{31271D5B-B40D-45F2-898B-D61F0B1B82E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73A41AAD-3763-4CD7-AF83-4C0971654BBF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{98C48DBD-1433-48C6-8761-997BB72F2AB5}"/>
   </bookViews>
@@ -3222,7 +3222,7 @@
   <dimension ref="A1:AB54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="W46" sqref="W46"/>
+      <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3559,7 +3559,7 @@
         <v>01/17/2016</v>
       </c>
       <c r="T4" s="2" t="str">
-        <f t="shared" ref="T4:T53" si="6">TEXT(T$2+(G3*7),"mm/dd/yyyy")</f>
+        <f t="shared" ref="T4:T52" si="6">TEXT(T$2+(G3*7),"mm/dd/yyyy")</f>
         <v>01/08/2017</v>
       </c>
       <c r="U4" s="2" t="str">
@@ -7615,7 +7615,7 @@
         <v>46</v>
       </c>
       <c r="M47">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N47">
         <v>46</v>
@@ -7711,7 +7711,7 @@
         <v>47</v>
       </c>
       <c r="M48">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N48">
         <v>47</v>
@@ -7762,7 +7762,7 @@
       </c>
       <c r="Z48" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>11/12/2023</v>
+        <v>11/19/2023</v>
       </c>
       <c r="AA48" s="2" t="str">
         <f t="shared" si="13"/>
@@ -7804,7 +7804,7 @@
         <v>48</v>
       </c>
       <c r="M49">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N49">
         <v>48</v>
@@ -7855,7 +7855,7 @@
       </c>
       <c r="Z49" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>11/19/2023</v>
+        <v>11/26/2023</v>
       </c>
       <c r="AA49" s="2" t="str">
         <f t="shared" si="13"/>
@@ -7948,7 +7948,7 @@
       </c>
       <c r="Z50" s="2" t="str">
         <f t="shared" si="12"/>
-        <v>11/26/2023</v>
+        <v>12/03/2023</v>
       </c>
       <c r="AA50" s="2" t="str">
         <f t="shared" si="13"/>
@@ -8040,7 +8040,7 @@
         <v>12/04/2022</v>
       </c>
       <c r="Z51" s="2" t="str">
-        <f t="shared" si="12"/>
+        <f>TEXT(Z$2+(M50*7),"mm/dd/yyyy")</f>
         <v>12/10/2023</v>
       </c>
       <c r="AA51" s="2" t="str">

</xml_diff>